<commit_message>
Add heaven gate table data structure and UI windows
</commit_message>
<xml_diff>
--- a/Documents/Project Manage/12-Month Programmer Calendar.xlsx
+++ b/Documents/Project Manage/12-Month Programmer Calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cookie/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GithubProjects\Hippocampus\Documents\Project Manage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECE3BB66-C098-954A-8B31-05E57EA651F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2F7098-ECEC-42B7-BB8F-03305BAED9AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38520" yWindow="3100" windowWidth="27740" windowHeight="15180" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JANUARY" sheetId="2" r:id="rId1"/>
@@ -36,6 +36,12 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -753,13 +759,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
@@ -770,7 +776,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>12</v>
       </c>
@@ -788,7 +794,7 @@
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="7">
         <f ca="1">CalendarYear</f>
         <v>2019</v>
@@ -800,7 +806,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -809,7 +815,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -839,7 +845,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+1</f>
         <v>43465</v>
@@ -869,7 +875,7 @@
         <v>43471</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -878,7 +884,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+8</f>
         <v>43472</v>
@@ -908,7 +914,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -919,7 +925,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+15</f>
         <v>43479</v>
@@ -949,7 +955,7 @@
         <v>43485</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -958,7 +964,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+22</f>
         <v>43486</v>
@@ -988,7 +994,7 @@
         <v>43492</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -997,7 +1003,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+29</f>
         <v>43493</v>
@@ -1027,7 +1033,7 @@
         <v>43499</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1036,7 +1042,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="13">
         <f t="array" aca="1" ref="B16:H16" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+36</f>
         <v>43500</v>
@@ -1066,7 +1072,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -1111,13 +1117,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -1134,7 +1140,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1143,7 +1149,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -1173,7 +1179,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+1</f>
         <v>43738</v>
@@ -1203,7 +1209,7 @@
         <v>43744</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1212,7 +1218,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+8</f>
         <v>43745</v>
@@ -1242,7 +1248,7 @@
         <v>43751</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1251,7 +1257,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+15</f>
         <v>43752</v>
@@ -1281,7 +1287,7 @@
         <v>43758</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -1290,7 +1296,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+22</f>
         <v>43759</v>
@@ -1320,7 +1326,7 @@
         <v>43765</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1329,7 +1335,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+29</f>
         <v>43766</v>
@@ -1359,7 +1365,7 @@
         <v>43772</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1368,7 +1374,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+36</f>
         <v>43773</v>
@@ -1398,7 +1404,7 @@
         <v>43779</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1438,13 +1444,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -1461,7 +1467,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
@@ -1470,7 +1476,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -1500,7 +1506,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+1</f>
         <v>43766</v>
@@ -1530,7 +1536,7 @@
         <v>43772</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1539,7 +1545,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+8</f>
         <v>43773</v>
@@ -1569,7 +1575,7 @@
         <v>43779</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1578,7 +1584,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+15</f>
         <v>43780</v>
@@ -1608,7 +1614,7 @@
         <v>43786</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -1617,7 +1623,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+22</f>
         <v>43787</v>
@@ -1647,7 +1653,7 @@
         <v>43793</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1656,7 +1662,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+29</f>
         <v>43794</v>
@@ -1686,7 +1692,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1695,7 +1701,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+36</f>
         <v>43801</v>
@@ -1725,7 +1731,7 @@
         <v>43807</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1764,16 +1770,16 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -1790,7 +1796,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1799,7 +1805,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -1829,7 +1835,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+1</f>
         <v>43794</v>
@@ -1859,7 +1865,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1868,7 +1874,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+8</f>
         <v>43801</v>
@@ -1898,7 +1904,7 @@
         <v>43807</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="210" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="210" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1913,7 +1919,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+15</f>
         <v>43808</v>
@@ -1943,7 +1949,7 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="237" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="237" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
         <v>42</v>
       </c>
@@ -1966,7 +1972,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+22</f>
         <v>43815</v>
@@ -1996,7 +2002,7 @@
         <v>43821</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>46</v>
       </c>
@@ -2019,7 +2025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+29</f>
         <v>43822</v>
@@ -2049,7 +2055,7 @@
         <v>43828</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="86" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="86.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>40</v>
       </c>
@@ -2072,7 +2078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+36</f>
         <v>43829</v>
@@ -2102,7 +2108,7 @@
         <v>43835</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="86" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="86.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
         <v>40</v>
       </c>
@@ -2146,13 +2152,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
         <v>2019</v>
@@ -2165,7 +2171,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2174,7 +2180,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -2204,7 +2210,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+1</f>
         <v>43493</v>
@@ -2234,7 +2240,7 @@
         <v>43499</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2243,7 +2249,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+8</f>
         <v>43500</v>
@@ -2273,7 +2279,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2282,7 +2288,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+15</f>
         <v>43507</v>
@@ -2312,7 +2318,7 @@
         <v>43513</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -2321,7 +2327,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+22</f>
         <v>43514</v>
@@ -2351,7 +2357,7 @@
         <v>43520</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -2360,7 +2366,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+29</f>
         <v>43521</v>
@@ -2390,7 +2396,7 @@
         <v>43527</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -2399,7 +2405,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+36</f>
         <v>43528</v>
@@ -2429,7 +2435,7 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -2469,13 +2475,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
         <v>2019</v>
@@ -2491,7 +2497,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
@@ -2500,7 +2506,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -2530,7 +2536,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+1</f>
         <v>43521</v>
@@ -2560,7 +2566,7 @@
         <v>43527</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2569,7 +2575,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+8</f>
         <v>43528</v>
@@ -2599,7 +2605,7 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2608,7 +2614,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+15</f>
         <v>43535</v>
@@ -2638,7 +2644,7 @@
         <v>43541</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -2647,7 +2653,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+22</f>
         <v>43542</v>
@@ -2677,7 +2683,7 @@
         <v>43548</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -2686,7 +2692,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+29</f>
         <v>43549</v>
@@ -2716,7 +2722,7 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -2725,7 +2731,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+36</f>
         <v>43556</v>
@@ -2755,7 +2761,7 @@
         <v>43562</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -2795,13 +2801,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
         <v>2019</v>
@@ -2817,7 +2823,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2826,7 +2832,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -2856,7 +2862,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+1</f>
         <v>43556</v>
@@ -2886,7 +2892,7 @@
         <v>43562</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2895,7 +2901,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+8</f>
         <v>43563</v>
@@ -2925,7 +2931,7 @@
         <v>43569</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2934,7 +2940,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+15</f>
         <v>43570</v>
@@ -2964,7 +2970,7 @@
         <v>43576</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -2973,7 +2979,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+22</f>
         <v>43577</v>
@@ -3003,7 +3009,7 @@
         <v>43583</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3012,7 +3018,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+29</f>
         <v>43584</v>
@@ -3042,7 +3048,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -3051,7 +3057,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+36</f>
         <v>43591</v>
@@ -3081,7 +3087,7 @@
         <v>43597</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -3121,13 +3127,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -3144,7 +3150,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -3153,7 +3159,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -3183,7 +3189,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+1</f>
         <v>43584</v>
@@ -3213,7 +3219,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -3222,7 +3228,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+8</f>
         <v>43591</v>
@@ -3252,7 +3258,7 @@
         <v>43597</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3261,7 +3267,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+15</f>
         <v>43598</v>
@@ -3291,7 +3297,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -3300,7 +3306,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+22</f>
         <v>43605</v>
@@ -3330,7 +3336,7 @@
         <v>43611</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3339,7 +3345,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+29</f>
         <v>43612</v>
@@ -3369,7 +3375,7 @@
         <v>43618</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -3378,7 +3384,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+36</f>
         <v>43619</v>
@@ -3408,7 +3414,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -3448,13 +3454,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -3471,7 +3477,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
@@ -3480,7 +3486,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -3510,7 +3516,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+1</f>
         <v>43612</v>
@@ -3540,7 +3546,7 @@
         <v>43618</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -3549,7 +3555,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+8</f>
         <v>43619</v>
@@ -3579,7 +3585,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3588,7 +3594,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+15</f>
         <v>43626</v>
@@ -3618,7 +3624,7 @@
         <v>43632</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -3627,7 +3633,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+22</f>
         <v>43633</v>
@@ -3657,7 +3663,7 @@
         <v>43639</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3666,7 +3672,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+29</f>
         <v>43640</v>
@@ -3696,7 +3702,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -3705,7 +3711,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+36</f>
         <v>43647</v>
@@ -3735,7 +3741,7 @@
         <v>43653</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -3775,13 +3781,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -3798,7 +3804,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
@@ -3807,7 +3813,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -3837,7 +3843,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+1</f>
         <v>43647</v>
@@ -3867,7 +3873,7 @@
         <v>43653</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -3876,7 +3882,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+8</f>
         <v>43654</v>
@@ -3906,7 +3912,7 @@
         <v>43660</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3915,7 +3921,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+15</f>
         <v>43661</v>
@@ -3945,7 +3951,7 @@
         <v>43667</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -3954,7 +3960,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+22</f>
         <v>43668</v>
@@ -3984,7 +3990,7 @@
         <v>43674</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3993,7 +3999,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+29</f>
         <v>43675</v>
@@ -4023,7 +4029,7 @@
         <v>43681</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -4032,7 +4038,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+36</f>
         <v>43682</v>
@@ -4062,7 +4068,7 @@
         <v>43688</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -4102,13 +4108,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -4125,7 +4131,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
@@ -4134,7 +4140,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -4164,7 +4170,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+1</f>
         <v>43675</v>
@@ -4194,7 +4200,7 @@
         <v>43681</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -4203,7 +4209,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+8</f>
         <v>43682</v>
@@ -4233,7 +4239,7 @@
         <v>43688</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -4242,7 +4248,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+15</f>
         <v>43689</v>
@@ -4272,7 +4278,7 @@
         <v>43695</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -4281,7 +4287,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+22</f>
         <v>43696</v>
@@ -4311,7 +4317,7 @@
         <v>43702</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -4320,7 +4326,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+29</f>
         <v>43703</v>
@@ -4350,7 +4356,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -4359,7 +4365,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+36</f>
         <v>43710</v>
@@ -4389,7 +4395,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -4429,13 +4435,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="8" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="8" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -4452,7 +4458,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
@@ -4461,7 +4467,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -4491,7 +4497,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+1</f>
         <v>43703</v>
@@ -4521,7 +4527,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -4530,7 +4536,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+8</f>
         <v>43710</v>
@@ -4560,7 +4566,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -4569,7 +4575,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+15</f>
         <v>43717</v>
@@ -4599,7 +4605,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -4608,7 +4614,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+22</f>
         <v>43724</v>
@@ -4638,7 +4644,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -4647,7 +4653,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+29</f>
         <v>43731</v>
@@ -4677,7 +4683,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -4686,7 +4692,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+36</f>
         <v>43738</v>
@@ -4716,7 +4722,7 @@
         <v>43744</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>

</xml_diff>

<commit_message>
Update team manage file
</commit_message>
<xml_diff>
--- a/Documents/Project Manage/12-Month Programmer Calendar.xlsx
+++ b/Documents/Project Manage/12-Month Programmer Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GithubProjects\Hippocampus\Documents\Project Manage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2F7098-ECEC-42B7-BB8F-03305BAED9AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6B9B25-F831-4227-AF23-BCB0E8AAAEAC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>MAY</t>
   </si>
@@ -179,32 +179,26 @@
     <t>维航Editor，输出表格，锦泽，扬威</t>
   </si>
   <si>
-    <t>维航Editor，文字控制符，字体调整，调整字体大小，锦泽，扬威</t>
-  </si>
-  <si>
-    <t>维航Editor，文字控制符，对话中停顿，可以调整等待的时长，锦泽，扬威</t>
+    <t>维航Unity，声音系统，固定音量播放，锦泽，扬威</t>
+  </si>
+  <si>
+    <t>维航Unity，镜头控制，跟着角色移动，锦泽，扬威</t>
+  </si>
+  <si>
+    <t>维航Editor，剧情分支，选项编辑，实现label和jump，锦泽Unity，UI框架，提供显示提示框，对话框，选择框和漂浮选择框，扬威Unity，虚拟摇杆，角色在场景中可移动</t>
+  </si>
+  <si>
+    <t>维航，锦泽Unity，更新资源管理系统，提供对于UI和场景的接口，整合Addressable，扬威Unity，剧情数据结构，json读取，在UI上显示基础对话，只显示名字和内容</t>
+  </si>
+  <si>
+    <t>维航Editor，文字控制符，立绘的移动，选择移动的方式、和位移。Editor，文字控制符，立绘的移动，选择移动的方式、和位移，锦泽，扬威</t>
   </si>
   <si>
     <t>维航Editor，文字控制符，Tips功能
-Editor。Tips编辑功能。锦泽，扬威</t>
-  </si>
-  <si>
-    <t>维航Unity，声音系统，固定音量播放，锦泽，扬威</t>
-  </si>
-  <si>
-    <t>维航Unity，镜头控制，跟着角色移动，锦泽，扬威</t>
-  </si>
-  <si>
-    <t>维航Editor，剧情分支，选项编辑，实现label和jump，锦泽Unity，UI框架，提供显示提示框，对话框，选择框和漂浮选择框，扬威Unity，虚拟摇杆，角色在场景中可移动</t>
-  </si>
-  <si>
-    <t>维航，锦泽Unity，更新资源管理系统，提供对于UI和场景的接口，整合Addressable，扬威Unity，剧情数据结构，json读取，在UI上显示基础对话，只显示名字和内容</t>
-  </si>
-  <si>
-    <t>维航，锦泽Unity，图片资源管理，扬威</t>
-  </si>
-  <si>
-    <t>维航Editor，文字控制符，立绘的移动，选择移动的方式、和位移。Editor，文字控制符，立绘的移动，选择移动的方式、和位移，锦泽Unity，对话框打字机效果，扬威</t>
+Editor。Tips编辑功能。锦泽Unity，图片资源管理，Unity，对话框打字机效果，扬威</t>
+  </si>
+  <si>
+    <t>维航Editor，文字控制符，对话中停顿，可以调整等待的时长，锦泽，扬威Unity，剧情分支，选项，实现label和jump这两个node的功能</t>
   </si>
 </sst>
 </file>
@@ -1769,8 +1763,8 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1910,13 +1904,13 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>41</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1951,25 +1945,25 @@
     </row>
     <row r="9" spans="1:8" ht="237" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2004,10 +1998,10 @@
     </row>
     <row r="11" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Update MacOS flatform, Update project manage files
</commit_message>
<xml_diff>
--- a/Documents/Project Manage/12-Month Programmer Calendar.xlsx
+++ b/Documents/Project Manage/12-Month Programmer Calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GithubProjects\Hippocampus\Documents\Project Manage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cookie/Documents/UnityProjectFolder/Hippocampus/Documents/Project Manage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6B9B25-F831-4227-AF23-BCB0E8AAAEAC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F31D56D-4DC3-6A41-A96A-5FCDC1900F8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="480" windowWidth="28800" windowHeight="17540" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JANUARY" sheetId="2" r:id="rId1"/>
@@ -36,12 +36,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -753,13 +747,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
@@ -770,7 +764,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="11" t="s">
         <v>12</v>
       </c>
@@ -788,7 +782,7 @@
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7">
         <f ca="1">CalendarYear</f>
         <v>2019</v>
@@ -800,7 +794,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -809,7 +803,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -839,7 +833,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="13">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+1</f>
         <v>43465</v>
@@ -869,7 +863,7 @@
         <v>43471</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -878,7 +872,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="13">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+8</f>
         <v>43472</v>
@@ -908,7 +902,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -919,7 +913,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="13">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+15</f>
         <v>43479</v>
@@ -949,7 +943,7 @@
         <v>43485</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -958,7 +952,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="13">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+22</f>
         <v>43486</v>
@@ -988,7 +982,7 @@
         <v>43492</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -997,7 +991,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="13">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+29</f>
         <v>43493</v>
@@ -1027,7 +1021,7 @@
         <v>43499</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1036,7 +1030,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="13">
         <f t="array" aca="1" ref="B16:H16" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="M")+1)+36</f>
         <v>43500</v>
@@ -1066,7 +1060,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -1111,13 +1105,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -1134,7 +1128,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1143,7 +1137,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -1173,7 +1167,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+1</f>
         <v>43738</v>
@@ -1203,7 +1197,7 @@
         <v>43744</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1212,7 +1206,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+8</f>
         <v>43745</v>
@@ -1242,7 +1236,7 @@
         <v>43751</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1251,7 +1245,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+15</f>
         <v>43752</v>
@@ -1281,7 +1275,7 @@
         <v>43758</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -1290,7 +1284,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+22</f>
         <v>43759</v>
@@ -1320,7 +1314,7 @@
         <v>43765</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1329,7 +1323,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+29</f>
         <v>43766</v>
@@ -1359,7 +1353,7 @@
         <v>43772</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1368,7 +1362,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,10,1)-WEEKDAY(DATE(CalendarYear,10,1),(WeekStart="M")+1)+36</f>
         <v>43773</v>
@@ -1398,7 +1392,7 @@
         <v>43779</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1438,13 +1432,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -1461,7 +1455,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
@@ -1470,7 +1464,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -1500,7 +1494,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+1</f>
         <v>43766</v>
@@ -1530,7 +1524,7 @@
         <v>43772</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1539,7 +1533,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+8</f>
         <v>43773</v>
@@ -1569,7 +1563,7 @@
         <v>43779</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1578,7 +1572,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+15</f>
         <v>43780</v>
@@ -1608,7 +1602,7 @@
         <v>43786</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -1617,7 +1611,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+22</f>
         <v>43787</v>
@@ -1647,7 +1641,7 @@
         <v>43793</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -1656,7 +1650,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+29</f>
         <v>43794</v>
@@ -1686,7 +1680,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1695,7 +1689,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,11,1)-WEEKDAY(DATE(CalendarYear,11,1),(WeekStart="M")+1)+36</f>
         <v>43801</v>
@@ -1725,7 +1719,7 @@
         <v>43807</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1763,17 +1757,17 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="25.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -1790,7 +1784,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1799,7 +1793,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -1829,7 +1823,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+1</f>
         <v>43794</v>
@@ -1859,7 +1853,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -1868,7 +1862,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+8</f>
         <v>43801</v>
@@ -1898,7 +1892,7 @@
         <v>43807</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="210" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="210" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1913,7 +1907,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+15</f>
         <v>43808</v>
@@ -1943,7 +1937,7 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="237" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="237" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="15" t="s">
         <v>40</v>
       </c>
@@ -1966,7 +1960,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+22</f>
         <v>43815</v>
@@ -1996,7 +1990,7 @@
         <v>43821</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="15" t="s">
         <v>43</v>
       </c>
@@ -2019,7 +2013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+29</f>
         <v>43822</v>
@@ -2049,7 +2043,7 @@
         <v>43828</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="86.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="86" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="15" t="s">
         <v>40</v>
       </c>
@@ -2072,7 +2066,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,12,1)-WEEKDAY(DATE(CalendarYear,12,1),(WeekStart="M")+1)+36</f>
         <v>43829</v>
@@ -2102,7 +2096,7 @@
         <v>43835</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="86.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="86" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="15" t="s">
         <v>40</v>
       </c>
@@ -2146,13 +2140,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
         <v>2019</v>
@@ -2165,7 +2159,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2174,7 +2168,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -2204,7 +2198,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+1</f>
         <v>43493</v>
@@ -2234,7 +2228,7 @@
         <v>43499</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2243,7 +2237,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+8</f>
         <v>43500</v>
@@ -2273,7 +2267,7 @@
         <v>43506</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2282,7 +2276,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+15</f>
         <v>43507</v>
@@ -2312,7 +2306,7 @@
         <v>43513</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -2321,7 +2315,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+22</f>
         <v>43514</v>
@@ -2351,7 +2345,7 @@
         <v>43520</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -2360,7 +2354,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+29</f>
         <v>43521</v>
@@ -2390,7 +2384,7 @@
         <v>43527</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -2399,7 +2393,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,2,1)-WEEKDAY(DATE(CalendarYear,2,1),(WeekStart="M")+1)+36</f>
         <v>43528</v>
@@ -2429,7 +2423,7 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -2469,13 +2463,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
         <v>2019</v>
@@ -2491,7 +2485,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
@@ -2500,7 +2494,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -2530,7 +2524,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+1</f>
         <v>43521</v>
@@ -2560,7 +2554,7 @@
         <v>43527</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2569,7 +2563,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+8</f>
         <v>43528</v>
@@ -2599,7 +2593,7 @@
         <v>43534</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2608,7 +2602,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+15</f>
         <v>43535</v>
@@ -2638,7 +2632,7 @@
         <v>43541</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -2647,7 +2641,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+22</f>
         <v>43542</v>
@@ -2677,7 +2671,7 @@
         <v>43548</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -2686,7 +2680,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+29</f>
         <v>43549</v>
@@ -2716,7 +2710,7 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -2725,7 +2719,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,3,1)-WEEKDAY(DATE(CalendarYear,3,1),(WeekStart="M")+1)+36</f>
         <v>43556</v>
@@ -2755,7 +2749,7 @@
         <v>43562</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -2795,13 +2789,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
         <v>2019</v>
@@ -2817,7 +2811,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
@@ -2826,7 +2820,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -2856,7 +2850,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+1</f>
         <v>43556</v>
@@ -2886,7 +2880,7 @@
         <v>43562</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -2895,7 +2889,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+8</f>
         <v>43563</v>
@@ -2925,7 +2919,7 @@
         <v>43569</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2934,7 +2928,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+15</f>
         <v>43570</v>
@@ -2964,7 +2958,7 @@
         <v>43576</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -2973,7 +2967,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+22</f>
         <v>43577</v>
@@ -3003,7 +2997,7 @@
         <v>43583</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3012,7 +3006,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+29</f>
         <v>43584</v>
@@ -3042,7 +3036,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -3051,7 +3045,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,4,1)-WEEKDAY(DATE(CalendarYear,4,1),(WeekStart="M")+1)+36</f>
         <v>43591</v>
@@ -3081,7 +3075,7 @@
         <v>43597</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -3121,13 +3115,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -3144,7 +3138,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -3153,7 +3147,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -3183,7 +3177,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+1</f>
         <v>43584</v>
@@ -3213,7 +3207,7 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -3222,7 +3216,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+8</f>
         <v>43591</v>
@@ -3252,7 +3246,7 @@
         <v>43597</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3261,7 +3255,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+15</f>
         <v>43598</v>
@@ -3291,7 +3285,7 @@
         <v>43604</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -3300,7 +3294,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+22</f>
         <v>43605</v>
@@ -3330,7 +3324,7 @@
         <v>43611</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3339,7 +3333,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+29</f>
         <v>43612</v>
@@ -3369,7 +3363,7 @@
         <v>43618</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -3378,7 +3372,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,5,1)-WEEKDAY(DATE(CalendarYear,5,1),(WeekStart="M")+1)+36</f>
         <v>43619</v>
@@ -3408,7 +3402,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -3448,13 +3442,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -3471,7 +3465,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
@@ -3480,7 +3474,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -3510,7 +3504,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+1</f>
         <v>43612</v>
@@ -3540,7 +3534,7 @@
         <v>43618</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -3549,7 +3543,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+8</f>
         <v>43619</v>
@@ -3579,7 +3573,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3588,7 +3582,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+15</f>
         <v>43626</v>
@@ -3618,7 +3612,7 @@
         <v>43632</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -3627,7 +3621,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+22</f>
         <v>43633</v>
@@ -3657,7 +3651,7 @@
         <v>43639</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3666,7 +3660,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+29</f>
         <v>43640</v>
@@ -3696,7 +3690,7 @@
         <v>43646</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -3705,7 +3699,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,6,1)-WEEKDAY(DATE(CalendarYear,6,1),(WeekStart="M")+1)+36</f>
         <v>43647</v>
@@ -3735,7 +3729,7 @@
         <v>43653</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -3775,13 +3769,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -3798,7 +3792,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
@@ -3807,7 +3801,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -3837,7 +3831,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+1</f>
         <v>43647</v>
@@ -3867,7 +3861,7 @@
         <v>43653</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -3876,7 +3870,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+8</f>
         <v>43654</v>
@@ -3906,7 +3900,7 @@
         <v>43660</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3915,7 +3909,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+15</f>
         <v>43661</v>
@@ -3945,7 +3939,7 @@
         <v>43667</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -3954,7 +3948,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+22</f>
         <v>43668</v>
@@ -3984,7 +3978,7 @@
         <v>43674</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3993,7 +3987,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+29</f>
         <v>43675</v>
@@ -4023,7 +4017,7 @@
         <v>43681</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -4032,7 +4026,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,7,1)-WEEKDAY(DATE(CalendarYear,7,1),(WeekStart="M")+1)+36</f>
         <v>43682</v>
@@ -4062,7 +4056,7 @@
         <v>43688</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -4102,13 +4096,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -4125,7 +4119,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
@@ -4134,7 +4128,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -4164,7 +4158,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+1</f>
         <v>43675</v>
@@ -4194,7 +4188,7 @@
         <v>43681</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -4203,7 +4197,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+8</f>
         <v>43682</v>
@@ -4233,7 +4227,7 @@
         <v>43688</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -4242,7 +4236,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+15</f>
         <v>43689</v>
@@ -4272,7 +4266,7 @@
         <v>43695</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -4281,7 +4275,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+22</f>
         <v>43696</v>
@@ -4311,7 +4305,7 @@
         <v>43702</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -4320,7 +4314,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+29</f>
         <v>43703</v>
@@ -4350,7 +4344,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -4359,7 +4353,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,8,1)-WEEKDAY(DATE(CalendarYear,8,1),(WeekStart="M")+1)+36</f>
         <v>43710</v>
@@ -4389,7 +4383,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -4429,13 +4423,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="8" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="7">
         <f ca="1">CalendarYear</f>
@@ -4452,7 +4446,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
@@ -4461,7 +4455,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="str">
         <f>WeekStart</f>
         <v>M</v>
@@ -4491,7 +4485,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4">
         <f t="array" aca="1" ref="B4:H4" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+1</f>
         <v>43703</v>
@@ -4521,7 +4515,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -4530,7 +4524,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4">
         <f t="array" aca="1" ref="B6:H6" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+8</f>
         <v>43710</v>
@@ -4560,7 +4554,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -4569,7 +4563,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4">
         <f t="array" aca="1" ref="B8:H8" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+15</f>
         <v>43717</v>
@@ -4599,7 +4593,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -4608,7 +4602,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4">
         <f t="array" aca="1" ref="B10:H10" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+22</f>
         <v>43724</v>
@@ -4638,7 +4632,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -4647,7 +4641,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4">
         <f t="array" aca="1" ref="B12:H12" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+29</f>
         <v>43731</v>
@@ -4677,7 +4671,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -4686,7 +4680,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <f t="array" aca="1" ref="B14:H14" ca="1">DaysAndWeeks+DATE(CalendarYear,9,1)-WEEKDAY(DATE(CalendarYear,9,1),(WeekStart="M")+1)+36</f>
         <v>43738</v>
@@ -4716,7 +4710,7 @@
         <v>43744</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>

</xml_diff>